<commit_message>
Updated bug fix list.
</commit_message>
<xml_diff>
--- a/Known Issues.xlsx
+++ b/Known Issues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cicic_000\Documents\ECS-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Screen</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Address field is truncated on save.</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -119,13 +128,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -435,75 +497,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="97" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -511,7 +604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -519,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -527,7 +620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -535,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -543,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -552,11 +645,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1">
-    <sortState ref="A2:B13">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D1"/>
+  <conditionalFormatting sqref="A1:D1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>INDIRECT("C"&amp;ROW())="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated list of known issues and bug fixes
</commit_message>
<xml_diff>
--- a/Known Issues.xlsx
+++ b/Known Issues.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cicic_000\Documents\ECS-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e6079583\Documents\_misc\ECS-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Screen</t>
   </si>
@@ -93,16 +93,38 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volunteer Type doesn't update when it is changed. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(NEW)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,23 +262,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -292,23 +297,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -461,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +460,7 @@
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="97" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -567,6 +556,12 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42871</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -575,6 +570,12 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
+        <v>42871</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -583,6 +584,12 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1">
+        <v>42871</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -618,6 +625,14 @@
       </c>
       <c r="B13" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the remaining two bugs
Fixed: Forgotten UserName - When data is entered into the form and submit is clicked, nothing happens.
Fixed: ResetPassword - When data is entered into the form and submit is clicked, nothing happens.
</commit_message>
<xml_diff>
--- a/Known Issues.xlsx
+++ b/Known Issues.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cicic_000\Documents\ECS-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e6079583\Documents\_misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Screen</t>
   </si>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,18 +111,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,16 +131,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,23 +248,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -305,23 +283,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,15 +533,19 @@
         <v>42892</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5">
+        <v>42898</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -652,15 +617,19 @@
         <v>42859</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5">
+        <v>42898</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>